<commit_message>
Added html and py files
</commit_message>
<xml_diff>
--- a/bacteria_archaea/marine/marine_prok_biomass_estimate.xlsx
+++ b/bacteria_archaea/marine/marine_prok_biomass_estimate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Parameter</t>
   </si>
@@ -40,12 +40,6 @@
     <t>Fraction of bacteria</t>
   </si>
   <si>
-    <t>0.2</t>
-  </si>
-  <si>
-    <t>0.8</t>
-  </si>
-  <si>
     <t>Cells</t>
   </si>
   <si>
@@ -55,10 +49,7 @@
     <t>Unitless</t>
   </si>
   <si>
-    <t>2.3</t>
-  </si>
-  <si>
-    <t>1.3</t>
+    <t>1.5</t>
   </si>
 </sst>
 </file>
@@ -444,10 +435,10 @@
         <v>1.23183254521155e+29</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>1.5</v>
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -458,7 +449,7 @@
         <v>11.2</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>1.4</v>
@@ -468,28 +459,28 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
+      <c r="B4">
+        <v>0.2</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>2.2</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
+      <c r="B5">
+        <v>0.8</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>1.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>